<commit_message>
separate regre suites for icdc
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Bento_E2E_Select-Single-Add-To-Cart.xlsx
+++ b/InputFiles/TC02_Bento_E2E_Select-Single-Add-To-Cart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55989B9-4282-4969-B9F6-FF54BEAE8106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A19F3C-9795-4DA8-8788-42A9EEE06230}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>